<commit_message>
Cập nhật phân trang
</commit_message>
<xml_diff>
--- a/Services/Server/Server.API/wwwroot/Reports/LICHSUDIEMDANH.xlsx
+++ b/Services/Server/Server.API/wwwroot/Reports/LICHSUDIEMDANH.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUUHUY\Projects\AMMS_IOT_DIEMDANH\Services\Server\Server.API\wwwroot\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACS\KhachHang\AMMS_DiemDanhHocSinh\Services\Server\Server.API\wwwroot\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4295C10E-9923-4FF5-8F0A-E49BCB35CA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888FF018-1EA7-49ED-9320-812E11DEBF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Items">Report1!$A$7:$J$8</definedName>
+    <definedName name="Items">Report1!$A$7:$K$8</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>(Ký, Ghi rõ họ tên)</t>
   </si>
@@ -49,36 +49,12 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Index</t>
-  </si>
-  <si>
-    <t>Student Code</t>
-  </si>
-  <si>
-    <t>Student Name</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Section</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>{{item.StudentCode}}</t>
   </si>
   <si>
     <t>{{item.StudentName}}</t>
   </si>
   <si>
-    <t>DeviceIp</t>
-  </si>
-  <si>
     <t>{{item.EventTime}}</t>
   </si>
   <si>
@@ -91,23 +67,54 @@
     <t>{{item.TAMessage}}</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>{{item.ClassCode}}</t>
-  </si>
-  <si>
     <t>{{item.DeviceIP}}</t>
+  </si>
+  <si>
+    <t>Stt</t>
+  </si>
+  <si>
+    <t>Mã học sinh</t>
+  </si>
+  <si>
+    <t>Họ tên</t>
+  </si>
+  <si>
+    <t>Lớp</t>
+  </si>
+  <si>
+    <t>Thiết bị</t>
+  </si>
+  <si>
+    <t>Thời gian điểm danh</t>
+  </si>
+  <si>
+    <t>Buổi</t>
+  </si>
+  <si>
+    <t>Sự kiện</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>{{item.ClassName}}</t>
+  </si>
+  <si>
+    <t>Trường</t>
+  </si>
+  <si>
+    <t>{{item.OrganizationName}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-1010409]General"/>
     <numFmt numFmtId="165" formatCode="[$-1010409]#,##0;\-#,##0"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -254,7 +261,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -286,6 +293,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -626,10 +636,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:K13"/>
+  <dimension ref="B1:L13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:J10"/>
+      <selection activeCell="C3" sqref="C3:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -638,75 +648,79 @@
     <col min="2" max="2" width="10.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" style="2" customWidth="1"/>
-    <col min="8" max="9" width="14.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="32.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="2.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="15" width="21.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="6" width="22.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="2" customWidth="1"/>
+    <col min="9" max="10" width="14.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="2.28515625" style="2" hidden="1" customWidth="1"/>
+    <col min="13" max="16" width="21.7109375" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="2:11" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="2:12" ht="19.5" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="2:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="2:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="2:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="2:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -717,68 +731,75 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="2:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="2:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>19</v>
+      <c r="F7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -789,8 +810,9 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -801,36 +823,39 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="1"/>
+      <c r="H10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="1"/>
+      <c r="H11" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="2:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="2:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -841,8 +866,9 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -853,16 +879,17 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="D2:K2"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="H4:K4"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0" top="0.19685039370078741" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="46" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Xuất báo cáo hs
</commit_message>
<xml_diff>
--- a/Services/Server/Server.API/wwwroot/Reports/LICHSUDIEMDANH.xlsx
+++ b/Services/Server/Server.API/wwwroot/Reports/LICHSUDIEMDANH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACS\KhachHang\AMMS_DiemDanhHocSinh\Services\Server\Server.API\wwwroot\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888FF018-1EA7-49ED-9320-812E11DEBF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7037C4C-F903-4074-9694-F29B04B17272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Report1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report1!$B$6:$K$6</definedName>
     <definedName name="Items">Report1!$A$7:$K$8</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -116,7 +117,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -124,19 +125,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -173,6 +161,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -271,52 +265,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="20" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" readingOrder="1"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -639,7 +633,7 @@
   <dimension ref="B1:L13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:K3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -785,7 +779,7 @@
       <c r="G7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>10</v>
       </c>
       <c r="I7" s="7" t="s">
@@ -794,7 +788,7 @@
       <c r="J7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="L7" s="1"/>
@@ -882,6 +876,7 @@
       <c r="L13" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="B6:K6" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="H10:K10"/>
     <mergeCell ref="H11:K11"/>

</xml_diff>